<commit_message>
Python scripts for a few
</commit_message>
<xml_diff>
--- a/RPAAirAndOceanCarrierStatuses.xlsx
+++ b/RPAAirAndOceanCarrierStatuses.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
+    <workbookView minimized="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Truckers " sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="173">
   <si>
     <t>V-00181--ITG TRANSPORTATION SERVICES INC</t>
   </si>
@@ -1796,8 +1796,8 @@
   <dimension ref="A1:X45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
+      <pane ySplit="3" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1960,7 +1960,7 @@
       </c>
       <c r="U5">
         <f>COUNTIF(F4:F45, "script done")</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="V5">
         <f>COUNTIF(F4:F45, "script in progress")</f>
@@ -1972,7 +1972,7 @@
       </c>
       <c r="X5">
         <f>ROWS(F4:F45)-U5-V5-W5</f>
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
@@ -2229,7 +2229,9 @@
       <c r="E22" s="28" t="s">
         <v>169</v>
       </c>
-      <c r="F22" s="27"/>
+      <c r="F22" s="27" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
@@ -2297,7 +2299,9 @@
       <c r="E27" s="28" t="s">
         <v>169</v>
       </c>
-      <c r="F27" s="27"/>
+      <c r="F27" s="27" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="3">

</xml_diff>

<commit_message>
Implemented RPA for a few and a few need to be fixed
</commit_message>
<xml_diff>
--- a/RPAAirAndOceanCarrierStatuses.xlsx
+++ b/RPAAirAndOceanCarrierStatuses.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pvanausdeln\Dropbox (Blume Global)\Documents\UiPath\AirCarrierRPA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Blume-proj\AirCarrierRPA\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="174">
   <si>
     <t>V-00181--ITG TRANSPORTATION SERVICES INC</t>
   </si>
@@ -560,6 +560,9 @@
   </si>
   <si>
     <t>RPA blocked by no site or site</t>
+  </si>
+  <si>
+    <t>RPA blocked by no data or site issue</t>
   </si>
 </sst>
 </file>
@@ -1796,8 +1799,8 @@
   <dimension ref="A1:X45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
+      <pane ySplit="3" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H26" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1928,7 +1931,7 @@
       <c r="F5" s="27"/>
       <c r="I5">
         <f>COUNTIF(D4:D45, "RPA done")</f>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J5">
         <f>COUNTIF(D4:D45,"RPA in progress")</f>
@@ -1936,11 +1939,11 @@
       </c>
       <c r="K5">
         <f>COUNTIF(D4:D45,"*RPA blocked*")</f>
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="L5">
         <f>ROWS(D4:D45)-K5-J5-I5</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="O5">
         <f>COUNTIF(E4:E45, "mapping done")</f>
@@ -2241,7 +2244,9 @@
         <v>73</v>
       </c>
       <c r="C23" s="2"/>
-      <c r="D23" s="27"/>
+      <c r="D23" s="27" t="s">
+        <v>173</v>
+      </c>
       <c r="E23" s="28"/>
       <c r="F23" s="27"/>
     </row>
@@ -2281,7 +2286,9 @@
         <v>76</v>
       </c>
       <c r="C26" s="2"/>
-      <c r="D26" s="27"/>
+      <c r="D26" s="27" t="s">
+        <v>161</v>
+      </c>
       <c r="E26" s="28"/>
       <c r="F26" s="27"/>
     </row>
@@ -2393,7 +2400,9 @@
         <v>83</v>
       </c>
       <c r="C33" s="2"/>
-      <c r="D33" s="27"/>
+      <c r="D33" s="27" t="s">
+        <v>156</v>
+      </c>
       <c r="E33" s="28"/>
       <c r="F33" s="27"/>
     </row>
@@ -2405,7 +2414,9 @@
         <v>84</v>
       </c>
       <c r="C34" s="2"/>
-      <c r="D34" s="27"/>
+      <c r="D34" s="27" t="s">
+        <v>157</v>
+      </c>
       <c r="E34" s="28"/>
       <c r="F34" s="27"/>
     </row>

</xml_diff>

<commit_message>
Script for united cargo
</commit_message>
<xml_diff>
--- a/RPAAirAndOceanCarrierStatuses.xlsx
+++ b/RPAAirAndOceanCarrierStatuses.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pvanausdeln\Dropbox (Blume Global)\Documents\UiPath\AirCarrierRPA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Blume-proj\AirCarrierRPA\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="173">
   <si>
     <t>V-00181--ITG TRANSPORTATION SERVICES INC</t>
   </si>
@@ -1796,8 +1796,8 @@
   <dimension ref="A1:X45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F44" sqref="F44"/>
+      <pane ySplit="3" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1960,7 +1960,7 @@
       </c>
       <c r="U5">
         <f>COUNTIF(F4:F45, "script done")</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="V5">
         <f>COUNTIF(F4:F45, "script in progress")</f>
@@ -1972,7 +1972,7 @@
       </c>
       <c r="X5">
         <f>ROWS(F4:F45)-U5-V5-W5</f>
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
@@ -2577,7 +2577,9 @@
       <c r="E44" s="28" t="s">
         <v>168</v>
       </c>
-      <c r="F44" s="27"/>
+      <c r="F44" s="27" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="3">

</xml_diff>

<commit_message>
more mappings and status updates
</commit_message>
<xml_diff>
--- a/RPAAirAndOceanCarrierStatuses.xlsx
+++ b/RPAAirAndOceanCarrierStatuses.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Blume-proj\AirCarrierRPA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pvanausdeln\Dropbox (Blume Global)\Documents\UiPath\AirCarrierRPA\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="173">
   <si>
     <t>V-00181--ITG TRANSPORTATION SERVICES INC</t>
   </si>
@@ -1796,8 +1796,8 @@
   <dimension ref="A1:X45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F45" sqref="F45"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1944,7 +1944,7 @@
       </c>
       <c r="O5">
         <f>COUNTIF(E4:E45, "mapping done")</f>
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="P5">
         <f>COUNTIF(E4:E45, "mapping in progress")</f>
@@ -1956,7 +1956,7 @@
       </c>
       <c r="R5">
         <f>ROWS(E4:E45)-O5-P5-Q5</f>
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="U5">
         <f>COUNTIF(F4:F45, "script done")</f>
@@ -2050,7 +2050,9 @@
       <c r="D10" s="27" t="s">
         <v>156</v>
       </c>
-      <c r="E10" s="28"/>
+      <c r="E10" s="28" t="s">
+        <v>168</v>
+      </c>
       <c r="F10" s="27"/>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
@@ -2064,7 +2066,9 @@
       <c r="D11" s="27" t="s">
         <v>156</v>
       </c>
-      <c r="E11" s="28"/>
+      <c r="E11" s="28" t="s">
+        <v>168</v>
+      </c>
       <c r="F11" s="27"/>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
@@ -2078,7 +2082,9 @@
       <c r="D12" s="27" t="s">
         <v>156</v>
       </c>
-      <c r="E12" s="28"/>
+      <c r="E12" s="28" t="s">
+        <v>168</v>
+      </c>
       <c r="F12" s="27"/>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
@@ -2106,7 +2112,9 @@
       <c r="D14" s="27" t="s">
         <v>156</v>
       </c>
-      <c r="E14" s="28"/>
+      <c r="E14" s="28" t="s">
+        <v>168</v>
+      </c>
       <c r="F14" s="27"/>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
@@ -2120,7 +2128,9 @@
       <c r="D15" s="27" t="s">
         <v>156</v>
       </c>
-      <c r="E15" s="28"/>
+      <c r="E15" s="28" t="s">
+        <v>168</v>
+      </c>
       <c r="F15" s="27"/>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
@@ -2528,7 +2538,9 @@
       <c r="D41" s="27" t="s">
         <v>156</v>
       </c>
-      <c r="E41" s="28"/>
+      <c r="E41" s="28" t="s">
+        <v>168</v>
+      </c>
       <c r="F41" s="27"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -2542,7 +2554,9 @@
       <c r="D42" s="27" t="s">
         <v>156</v>
       </c>
-      <c r="E42" s="28"/>
+      <c r="E42" s="28" t="s">
+        <v>168</v>
+      </c>
       <c r="F42" s="27"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Tampa script in progress
</commit_message>
<xml_diff>
--- a/RPAAirAndOceanCarrierStatuses.xlsx
+++ b/RPAAirAndOceanCarrierStatuses.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pvanausdeln\Dropbox (Blume Global)\Documents\UiPath\AirCarrierRPA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pvanausdeln\OneDrive - Blume Global\UiPath\AirCarrierRPA\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="174">
   <si>
     <t>V-00181--ITG TRANSPORTATION SERVICES INC</t>
   </si>
@@ -560,6 +560,9 @@
   </si>
   <si>
     <t>RPA blocked by no site</t>
+  </si>
+  <si>
+    <t>script in progress</t>
   </si>
 </sst>
 </file>
@@ -1797,7 +1800,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
+      <selection pane="bottomLeft" activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1964,7 +1967,7 @@
       </c>
       <c r="V5">
         <f>COUNTIF(F4:F45, "script in progress")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W5">
         <f>COUNTIF(F4:F45, "*script blocked*")</f>
@@ -1972,7 +1975,7 @@
       </c>
       <c r="X5">
         <f>ROWS(F4:F45)-U5-V5-W5</f>
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
@@ -2541,7 +2544,9 @@
       <c r="E41" s="28" t="s">
         <v>168</v>
       </c>
-      <c r="F41" s="27"/>
+      <c r="F41" s="27" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
@@ -2557,7 +2562,9 @@
       <c r="E42" s="28" t="s">
         <v>168</v>
       </c>
-      <c r="F42" s="27"/>
+      <c r="F42" s="27" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="3">

</xml_diff>

<commit_message>
British script in progress
</commit_message>
<xml_diff>
--- a/RPAAirAndOceanCarrierStatuses.xlsx
+++ b/RPAAirAndOceanCarrierStatuses.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="174">
   <si>
     <t>V-00181--ITG TRANSPORTATION SERVICES INC</t>
   </si>
@@ -1800,7 +1800,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F43" sqref="F43"/>
+      <selection pane="bottomLeft" activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1967,7 +1967,7 @@
       </c>
       <c r="V5">
         <f>COUNTIF(F4:F45, "script in progress")</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="W5">
         <f>COUNTIF(F4:F45, "*script blocked*")</f>
@@ -1975,7 +1975,7 @@
       </c>
       <c r="X5">
         <f>ROWS(F4:F45)-U5-V5-W5</f>
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
@@ -2118,7 +2118,9 @@
       <c r="E14" s="28" t="s">
         <v>168</v>
       </c>
-      <c r="F14" s="27"/>
+      <c r="F14" s="27" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
@@ -2134,7 +2136,9 @@
       <c r="E15" s="28" t="s">
         <v>168</v>
       </c>
-      <c r="F15" s="27"/>
+      <c r="F15" s="27" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="3">

</xml_diff>